<commit_message>
MAJ Excel : Sujet Infection + corrections
</commit_message>
<xml_diff>
--- a/res/MeFconditionnelle.xlsx
+++ b/res/MeFconditionnelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IUTtravail\cours\excel\cours20182019\captureexcels2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IUTtravail\cours\excel\Excel20192020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C0E70E46-ECC4-45D9-9870-AA299A708E96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A6F3C25-064B-46B1-95C6-6C708C0A3E59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E32F2BEA-281A-428C-8829-045D2759FCD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E32F2BEA-281A-428C-8829-045D2759FCD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -192,167 +192,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">

</xml_diff>